<commit_message>
Zermolo Model in excel / calc.
</commit_message>
<xml_diff>
--- a/zermelo-model.xlsx
+++ b/zermelo-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Zermelo Model CT NYM1924" sheetId="1" state="visible" r:id="rId3"/>
@@ -18,6 +18,10 @@
     <definedName function="false" hidden="false" name="solver_adj_0" vbProcedure="false">'test_-1'!$d$25:$d$35</definedName>
     <definedName function="false" hidden="true" name="solver_adj_1" vbProcedure="false">nym!$d$71:$d$127</definedName>
     <definedName function="false" hidden="false" name="solver_adj_10" vbProcedure="false">test!$d$25:$d$35</definedName>
+    <definedName function="false" hidden="false" name="solver_adj_11" vbProcedure="false">'nym_-1'!$d$25:$d$35</definedName>
+    <definedName function="false" hidden="false" name="solver_adj_12" vbProcedure="false">'test_-1'!$d$25:$d$35</definedName>
+    <definedName function="false" hidden="false" name="solver_adj_13" vbProcedure="false">nym!$d$25:$d$35</definedName>
+    <definedName function="false" hidden="false" name="solver_adj_14" vbProcedure="false">test!$d$25:$d$35</definedName>
     <definedName function="false" hidden="true" name="solver_adj_2" vbProcedure="false">test!$d$71:$d$127</definedName>
     <definedName function="false" hidden="false" name="solver_adj_3" vbProcedure="false">'nym_-1'!$d$25:$d$35</definedName>
     <definedName function="false" hidden="false" name="solver_adj_4" vbProcedure="false">'test_-1'!$d$25:$d$35</definedName>
@@ -31,6 +35,10 @@
     <definedName function="false" hidden="false" name="solver_cvg_1" vbProcedure="false">0.0001</definedName>
     <definedName function="false" hidden="false" name="solver_cvg_10" vbProcedure="false">0.0001</definedName>
     <definedName function="false" hidden="false" name="solver_cvg_11" vbProcedure="false">0.0001</definedName>
+    <definedName function="false" hidden="false" name="solver_cvg_12" vbProcedure="false">0.0001</definedName>
+    <definedName function="false" hidden="false" name="solver_cvg_13" vbProcedure="false">0.0001</definedName>
+    <definedName function="false" hidden="false" name="solver_cvg_14" vbProcedure="false">0.0001</definedName>
+    <definedName function="false" hidden="false" name="solver_cvg_15" vbProcedure="false">0.0001</definedName>
     <definedName function="false" hidden="true" name="solver_cvg_2" vbProcedure="false">0.0001</definedName>
     <definedName function="false" hidden="true" name="solver_cvg_3" vbProcedure="false">0.0001</definedName>
     <definedName function="false" hidden="false" name="solver_cvg_4" vbProcedure="false">0.0001</definedName>
@@ -44,6 +52,10 @@
     <definedName function="false" hidden="false" name="solver_drv_1" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_drv_10" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_drv_11" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_drv_12" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_drv_13" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_drv_14" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_drv_15" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_drv_2" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_drv_3" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_drv_4" vbProcedure="false">1</definedName>
@@ -59,6 +71,10 @@
     <definedName function="false" hidden="false" name="solver_est_1" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_est_10" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_est_11" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_est_12" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_est_13" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_est_14" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_est_15" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_est_2" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_est_3" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_est_4" vbProcedure="false">1</definedName>
@@ -72,6 +88,10 @@
     <definedName function="false" hidden="false" name="solver_itr_1" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="false" name="solver_itr_10" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="false" name="solver_itr_11" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_itr_12" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_itr_13" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_itr_14" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_itr_15" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="true" name="solver_itr_2" vbProcedure="false">2147483647</definedName>
     <definedName function="false" hidden="true" name="solver_itr_3" vbProcedure="false">2147483647</definedName>
     <definedName function="false" hidden="false" name="solver_itr_4" vbProcedure="false">100</definedName>
@@ -84,6 +104,10 @@
     <definedName function="false" hidden="false" name="solver_lhs1_0" vbProcedure="false">'test_-1'!$d$36</definedName>
     <definedName function="false" hidden="true" name="solver_lhs1_1" vbProcedure="false">nym!$d$128</definedName>
     <definedName function="false" hidden="false" name="solver_lhs1_10" vbProcedure="false">test!$d$36</definedName>
+    <definedName function="false" hidden="false" name="solver_lhs1_11" vbProcedure="false">'nym_-1'!$d$36</definedName>
+    <definedName function="false" hidden="false" name="solver_lhs1_12" vbProcedure="false">'test_-1'!$d$36</definedName>
+    <definedName function="false" hidden="false" name="solver_lhs1_13" vbProcedure="false">nym!$d$36</definedName>
+    <definedName function="false" hidden="false" name="solver_lhs1_14" vbProcedure="false">test!$d$36</definedName>
     <definedName function="false" hidden="true" name="solver_lhs1_2" vbProcedure="false">test!$d$128</definedName>
     <definedName function="false" hidden="false" name="solver_lhs1_3" vbProcedure="false">'nym_-1'!$d$36</definedName>
     <definedName function="false" hidden="false" name="solver_lhs1_4" vbProcedure="false">'test_-1'!$d$36</definedName>
@@ -97,6 +121,10 @@
     <definedName function="false" hidden="false" name="solver_lin" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_lin_0" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_lin_1" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_lin_10" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_lin_11" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_lin_12" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_lin_13" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_lin_2" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_lin_3" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_lin_4" vbProcedure="false">2</definedName>
@@ -118,6 +146,10 @@
     <definedName function="false" hidden="false" name="solver_neg_1" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_neg_10" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_neg_11" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_neg_12" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_neg_13" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_neg_14" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_neg_15" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_neg_2" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_neg_3" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_neg_4" vbProcedure="false">2</definedName>
@@ -133,6 +165,10 @@
     <definedName function="false" hidden="false" name="solver_num_1" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_num_10" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_num_11" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_num_12" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_num_13" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_num_14" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_num_15" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_num_2" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_num_3" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_num_4" vbProcedure="false">1</definedName>
@@ -146,6 +182,10 @@
     <definedName function="false" hidden="false" name="solver_nwt_1" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_nwt_10" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_nwt_11" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_nwt_12" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_nwt_13" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_nwt_14" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_nwt_15" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_nwt_2" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_nwt_3" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_nwt_4" vbProcedure="false">1</definedName>
@@ -158,6 +198,10 @@
     <definedName function="false" hidden="false" name="solver_opt_0" vbProcedure="false">'test_-1'!$o$54</definedName>
     <definedName function="false" hidden="true" name="solver_opt_1" vbProcedure="false">nym!$o$129</definedName>
     <definedName function="false" hidden="false" name="solver_opt_10" vbProcedure="false">test!$o$54</definedName>
+    <definedName function="false" hidden="false" name="solver_opt_11" vbProcedure="false">'nym_-1'!$o$54</definedName>
+    <definedName function="false" hidden="false" name="solver_opt_12" vbProcedure="false">'test_-1'!$o$54</definedName>
+    <definedName function="false" hidden="false" name="solver_opt_13" vbProcedure="false">nym!$o$54</definedName>
+    <definedName function="false" hidden="false" name="solver_opt_14" vbProcedure="false">test!$o$54</definedName>
     <definedName function="false" hidden="true" name="solver_opt_2" vbProcedure="false">test!$o$129</definedName>
     <definedName function="false" hidden="false" name="solver_opt_3" vbProcedure="false">'nym_-1'!$o$54</definedName>
     <definedName function="false" hidden="false" name="solver_opt_4" vbProcedure="false">'test_-1'!$o$54</definedName>
@@ -171,6 +215,10 @@
     <definedName function="false" hidden="false" name="solver_pre_1" vbProcedure="false">0.000001</definedName>
     <definedName function="false" hidden="false" name="solver_pre_10" vbProcedure="false">0.000001</definedName>
     <definedName function="false" hidden="false" name="solver_pre_11" vbProcedure="false">0.000001</definedName>
+    <definedName function="false" hidden="false" name="solver_pre_12" vbProcedure="false">0.000001</definedName>
+    <definedName function="false" hidden="false" name="solver_pre_13" vbProcedure="false">0.000001</definedName>
+    <definedName function="false" hidden="false" name="solver_pre_14" vbProcedure="false">0.000001</definedName>
+    <definedName function="false" hidden="false" name="solver_pre_15" vbProcedure="false">0.000001</definedName>
     <definedName function="false" hidden="true" name="solver_pre_2" vbProcedure="false">0.000001</definedName>
     <definedName function="false" hidden="true" name="solver_pre_3" vbProcedure="false">0.000001</definedName>
     <definedName function="false" hidden="false" name="solver_pre_4" vbProcedure="false">0.000001</definedName>
@@ -186,6 +234,10 @@
     <definedName function="false" hidden="false" name="solver_rel1_1" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_rel1_10" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_rel1_11" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_rel1_12" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_rel1_13" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_rel1_14" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_rel1_15" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_rel1_2" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_rel1_3" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_rel1_4" vbProcedure="false">2</definedName>
@@ -201,6 +253,10 @@
     <definedName function="false" hidden="false" name="solver_rhs1_1" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_rhs1_10" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_rhs1_11" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_rhs1_12" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_rhs1_13" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_rhs1_14" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_rhs1_15" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_rhs1_2" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_rhs1_3" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_rhs1_4" vbProcedure="false">1</definedName>
@@ -220,6 +276,10 @@
     <definedName function="false" hidden="false" name="solver_scl_1" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_scl_10" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_scl_11" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_scl_12" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_scl_13" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_scl_14" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_scl_15" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_scl_2" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_scl_3" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_scl_4" vbProcedure="false">2</definedName>
@@ -233,6 +293,10 @@
     <definedName function="false" hidden="false" name="solver_sho_1" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_sho_10" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_sho_11" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_sho_12" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_sho_13" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_sho_14" vbProcedure="false">2</definedName>
+    <definedName function="false" hidden="false" name="solver_sho_15" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_sho_2" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="true" name="solver_sho_3" vbProcedure="false">2</definedName>
     <definedName function="false" hidden="false" name="solver_sho_4" vbProcedure="false">2</definedName>
@@ -248,6 +312,10 @@
     <definedName function="false" hidden="false" name="solver_tim_1" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="false" name="solver_tim_10" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="false" name="solver_tim_11" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_tim_12" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_tim_13" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_tim_14" vbProcedure="false">100</definedName>
+    <definedName function="false" hidden="false" name="solver_tim_15" vbProcedure="false">100</definedName>
     <definedName function="false" hidden="true" name="solver_tim_2" vbProcedure="false">2147483647</definedName>
     <definedName function="false" hidden="true" name="solver_tim_3" vbProcedure="false">2147483647</definedName>
     <definedName function="false" hidden="false" name="solver_tim_4" vbProcedure="false">100</definedName>
@@ -261,6 +329,10 @@
     <definedName function="false" hidden="false" name="solver_tol_1" vbProcedure="false">0.05</definedName>
     <definedName function="false" hidden="false" name="solver_tol_10" vbProcedure="false">0.05</definedName>
     <definedName function="false" hidden="false" name="solver_tol_11" vbProcedure="false">0.05</definedName>
+    <definedName function="false" hidden="false" name="solver_tol_12" vbProcedure="false">0.05</definedName>
+    <definedName function="false" hidden="false" name="solver_tol_13" vbProcedure="false">0.05</definedName>
+    <definedName function="false" hidden="false" name="solver_tol_14" vbProcedure="false">0.05</definedName>
+    <definedName function="false" hidden="false" name="solver_tol_15" vbProcedure="false">0.05</definedName>
     <definedName function="false" hidden="true" name="solver_tol_2" vbProcedure="false">0.01</definedName>
     <definedName function="false" hidden="true" name="solver_tol_3" vbProcedure="false">0.01</definedName>
     <definedName function="false" hidden="false" name="solver_tol_4" vbProcedure="false">0.05</definedName>
@@ -274,6 +346,10 @@
     <definedName function="false" hidden="false" name="solver_typ_1" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_typ_10" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_typ_11" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_typ_12" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_typ_13" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_typ_14" vbProcedure="false">1</definedName>
+    <definedName function="false" hidden="false" name="solver_typ_15" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_typ_2" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="true" name="solver_typ_3" vbProcedure="false">1</definedName>
     <definedName function="false" hidden="false" name="solver_typ_4" vbProcedure="false">1</definedName>
@@ -287,6 +363,10 @@
     <definedName function="false" hidden="false" name="solver_val_1" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" name="solver_val_10" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" name="solver_val_11" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" name="solver_val_12" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" name="solver_val_13" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" name="solver_val_14" vbProcedure="false">0</definedName>
+    <definedName function="false" hidden="false" name="solver_val_15" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="true" name="solver_val_2" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="true" name="solver_val_3" vbProcedure="false">0</definedName>
     <definedName function="false" hidden="false" name="solver_val_4" vbProcedure="false">0</definedName>
@@ -300,6 +380,9 @@
     <definedName function="false" hidden="false" name="_xlnm.Print_Area" vbProcedure="false">'nym_-1'!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_0" vbProcedure="false">'test_-1'!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_1" vbProcedure="false">'nym_-1'!$a$1:$al$42</definedName>
+    <definedName function="false" hidden="false" name="_xlnm.Print_Area_10" vbProcedure="false">'test_-1'!$a$1:$al$42</definedName>
+    <definedName function="false" hidden="false" name="_xlnm.Print_Area_11" vbProcedure="false">nym!$a$1:$al$42</definedName>
+    <definedName function="false" hidden="false" name="_xlnm.Print_Area_12" vbProcedure="false">test!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_2" vbProcedure="false">'test_-1'!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_3" vbProcedure="false">nym!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_4" vbProcedure="false">test!$a$1:$al$42</definedName>
@@ -307,6 +390,7 @@
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_6" vbProcedure="false">'test_-1'!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_7" vbProcedure="false">nym!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" name="_xlnm.Print_Area_8" vbProcedure="false">test!$a$1:$al$42</definedName>
+    <definedName function="false" hidden="false" name="_xlnm.Print_Area_9" vbProcedure="false">'nym_-1'!$a$1:$al$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="solver_adj" vbProcedure="false">'Zermelo Model CT NYM1924'!$D$25:$D$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="solver_cvg" vbProcedure="false">0.0001</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="solver_drv" vbProcedure="false">1</definedName>
@@ -1381,7 +1465,7 @@
   </sheetPr>
   <dimension ref="A1:AL54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -5052,8 +5136,8 @@
   </sheetPr>
   <dimension ref="A1:BH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O38" activeCellId="0" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5270,7 +5354,7 @@
       </c>
       <c r="D7" s="15" t="n">
         <f aca="false">D25</f>
-        <v>3.84057122542288</v>
+        <v>1</v>
       </c>
       <c r="E7" s="19" t="n">
         <f aca="false">SUM(G7:I7)</f>
@@ -5454,7 +5538,7 @@
       </c>
       <c r="D8" s="15" t="n">
         <f aca="false">D26</f>
-        <v>2.60110529486542</v>
+        <v>1</v>
       </c>
       <c r="E8" s="19" t="n">
         <f aca="false">SUM(G8:I8)</f>
@@ -5638,7 +5722,7 @@
       </c>
       <c r="D9" s="15" t="n">
         <f aca="false">D27</f>
-        <v>1.49150646955304</v>
+        <v>1</v>
       </c>
       <c r="E9" s="19" t="n">
         <f aca="false">SUM(G9:I9)</f>
@@ -5822,7 +5906,7 @@
       </c>
       <c r="D10" s="15" t="n">
         <f aca="false">D28</f>
-        <v>1.21346351463835</v>
+        <v>1</v>
       </c>
       <c r="E10" s="19" t="n">
         <f aca="false">SUM(G10:I10)</f>
@@ -6006,7 +6090,7 @@
       </c>
       <c r="D11" s="15" t="n">
         <f aca="false">D29</f>
-        <v>1.09622034605353</v>
+        <v>1</v>
       </c>
       <c r="E11" s="19" t="n">
         <f aca="false">SUM(G11:I11)</f>
@@ -6190,7 +6274,7 @@
       </c>
       <c r="D12" s="15" t="n">
         <f aca="false">D30</f>
-        <v>0.990796706847064</v>
+        <v>1</v>
       </c>
       <c r="E12" s="19" t="n">
         <f aca="false">SUM(G12:I12)</f>
@@ -6374,7 +6458,7 @@
       </c>
       <c r="D13" s="15" t="n">
         <f aca="false">D31</f>
-        <v>0.895611500950775</v>
+        <v>1</v>
       </c>
       <c r="E13" s="19" t="n">
         <f aca="false">SUM(G13:I13)</f>
@@ -6558,7 +6642,7 @@
       </c>
       <c r="D14" s="15" t="n">
         <f aca="false">D32</f>
-        <v>0.659356578928798</v>
+        <v>1</v>
       </c>
       <c r="E14" s="19" t="n">
         <f aca="false">SUM(G14:I14)</f>
@@ -6742,7 +6826,7 @@
       </c>
       <c r="D15" s="15" t="n">
         <f aca="false">D33</f>
-        <v>0.533871781372612</v>
+        <v>1</v>
       </c>
       <c r="E15" s="19" t="n">
         <f aca="false">SUM(G15:I15)</f>
@@ -6926,7 +7010,7 @@
       </c>
       <c r="D16" s="15" t="n">
         <f aca="false">D34</f>
-        <v>0.478680132136038</v>
+        <v>1</v>
       </c>
       <c r="E16" s="19" t="n">
         <f aca="false">SUM(G16:I16)</f>
@@ -7110,7 +7194,7 @@
       </c>
       <c r="D17" s="15" t="n">
         <f aca="false">D35</f>
-        <v>0.337434583962304</v>
+        <v>1</v>
       </c>
       <c r="E17" s="19" t="n">
         <f aca="false">SUM(G17:I17)</f>
@@ -7529,7 +7613,7 @@
       <c r="F23" s="21"/>
       <c r="G23" s="22" t="n">
         <f aca="false" t="array" ref="G23:G23">SQRT(SUMSQ(D25:D35-G25:G35))</f>
-        <v>3.48447462258474E-008</v>
+        <v>1.13102334965379</v>
       </c>
       <c r="H23" s="23" t="n">
         <v>100</v>
@@ -7542,7 +7626,7 @@
       <c r="L23" s="20"/>
       <c r="O23" s="22" t="n">
         <f aca="false" t="array" ref="O23:O23">SQRT(SUMSQ(O7:O17-O25:O35))</f>
-        <v>1.42635456077999E-007</v>
+        <v>10.5830052442584</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7599,7 +7683,7 @@
         <v> Emanuel Lasker (Germany) </v>
       </c>
       <c r="D25" s="26" t="n">
-        <v>3.84057122542288</v>
+        <v>1</v>
       </c>
       <c r="E25" s="19" t="n">
         <f aca="false">E7</f>
@@ -7608,26 +7692,26 @@
       <c r="F25" s="19"/>
       <c r="G25" s="27" t="n">
         <f aca="false">M25/$M$36</f>
-        <v>3.84057126012645</v>
+        <v>1.68770913104735</v>
       </c>
       <c r="H25" s="15" t="n">
         <f aca="false">M25*H$23/$M$37</f>
-        <v>27.1636960310592</v>
+        <v>14.5454545454545</v>
       </c>
       <c r="I25" s="42" t="n">
         <f aca="false">LN(G25)*$I$23</f>
-        <v>233.758331066644</v>
+        <v>90.9190400281659</v>
       </c>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20" t="n">
         <f aca="false">D25*O7/O25</f>
-        <v>3.8405712579823</v>
+        <v>1.6</v>
       </c>
       <c r="O25" s="16" t="n">
         <f aca="false">SUM(P25:AK25)</f>
-        <v>15.9999998643559</v>
+        <v>10</v>
       </c>
       <c r="P25" s="28" t="n">
         <f aca="false">IF(AM7=0,0,$D25/($D25+INDEX($D$7:$D$17,AM7)))</f>
@@ -7635,43 +7719,43 @@
       </c>
       <c r="Q25" s="29" t="n">
         <f aca="false">IF(AN7=0,0,$D25/($D25+INDEX($D$7:$D$17,AN7)))</f>
-        <v>0.596206781468591</v>
+        <v>0.5</v>
       </c>
       <c r="R25" s="29" t="n">
         <f aca="false">IF(AO7=0,0,$D25/($D25+INDEX($D$7:$D$17,AO7)))</f>
-        <v>0.720276681084675</v>
+        <v>0.5</v>
       </c>
       <c r="S25" s="29" t="n">
         <f aca="false">IF(AP7=0,0,$D25/($D25+INDEX($D$7:$D$17,AP7)))</f>
-        <v>0.759902023423043</v>
+        <v>0.5</v>
       </c>
       <c r="T25" s="29" t="n">
         <f aca="false">IF(AQ7=0,0,$D25/($D25+INDEX($D$7:$D$17,AQ7)))</f>
-        <v>0.777948829683792</v>
+        <v>0.5</v>
       </c>
       <c r="U25" s="29" t="n">
         <f aca="false">IF(AR7=0,0,$D25/($D25+INDEX($D$7:$D$17,AR7)))</f>
-        <v>0.794924186951427</v>
+        <v>0.5</v>
       </c>
       <c r="V25" s="29" t="n">
         <f aca="false">IF(AS7=0,0,$D25/($D25+INDEX($D$7:$D$17,AS7)))</f>
-        <v>0.810900137791661</v>
+        <v>0.5</v>
       </c>
       <c r="W25" s="29" t="n">
         <f aca="false">IF(AT7=0,0,$D25/($D25+INDEX($D$7:$D$17,AT7)))</f>
-        <v>0.853473965006469</v>
+        <v>0.5</v>
       </c>
       <c r="X25" s="29" t="n">
         <f aca="false">IF(AU7=0,0,$D25/($D25+INDEX($D$7:$D$17,AU7)))</f>
-        <v>0.87795662658234</v>
+        <v>0.5</v>
       </c>
       <c r="Y25" s="29" t="n">
         <f aca="false">IF(AV7=0,0,$D25/($D25+INDEX($D$7:$D$17,AV7)))</f>
-        <v>0.889175208268831</v>
+        <v>0.5</v>
       </c>
       <c r="Z25" s="29" t="n">
         <f aca="false">IF(AW7=0,0,$D25/($D25+INDEX($D$7:$D$17,AW7)))</f>
-        <v>0.919235491917145</v>
+        <v>0.5</v>
       </c>
       <c r="AA25" s="29" t="n">
         <f aca="false">IF(AX7=0,0,$D25/($D25+INDEX($D$7:$D$17,AX7)))</f>
@@ -7679,43 +7763,43 @@
       </c>
       <c r="AB25" s="29" t="n">
         <f aca="false">IF(AY7=0,0,$D25/($D25+INDEX($D$7:$D$17,AY7)))</f>
-        <v>0.596206781468591</v>
+        <v>0.5</v>
       </c>
       <c r="AC25" s="29" t="n">
         <f aca="false">IF(AZ7=0,0,$D25/($D25+INDEX($D$7:$D$17,AZ7)))</f>
-        <v>0.720276681084675</v>
+        <v>0.5</v>
       </c>
       <c r="AD25" s="29" t="n">
         <f aca="false">IF(BA7=0,0,$D25/($D25+INDEX($D$7:$D$17,BA7)))</f>
-        <v>0.759902023423043</v>
+        <v>0.5</v>
       </c>
       <c r="AE25" s="29" t="n">
         <f aca="false">IF(BB7=0,0,$D25/($D25+INDEX($D$7:$D$17,BB7)))</f>
-        <v>0.777948829683792</v>
+        <v>0.5</v>
       </c>
       <c r="AF25" s="29" t="n">
         <f aca="false">IF(BC7=0,0,$D25/($D25+INDEX($D$7:$D$17,BC7)))</f>
-        <v>0.794924186951427</v>
+        <v>0.5</v>
       </c>
       <c r="AG25" s="29" t="n">
         <f aca="false">IF(BD7=0,0,$D25/($D25+INDEX($D$7:$D$17,BD7)))</f>
-        <v>0.810900137791661</v>
+        <v>0.5</v>
       </c>
       <c r="AH25" s="29" t="n">
         <f aca="false">IF(BE7=0,0,$D25/($D25+INDEX($D$7:$D$17,BE7)))</f>
-        <v>0.853473965006469</v>
+        <v>0.5</v>
       </c>
       <c r="AI25" s="29" t="n">
         <f aca="false">IF(BF7=0,0,$D25/($D25+INDEX($D$7:$D$17,BF7)))</f>
-        <v>0.87795662658234</v>
+        <v>0.5</v>
       </c>
       <c r="AJ25" s="29" t="n">
         <f aca="false">IF(BG7=0,0,$D25/($D25+INDEX($D$7:$D$17,BG7)))</f>
-        <v>0.889175208268831</v>
+        <v>0.5</v>
       </c>
       <c r="AK25" s="30" t="n">
         <f aca="false">IF(BH7=0,0,$D25/($D25+INDEX($D$7:$D$17,BH7)))</f>
-        <v>0.919235491917145</v>
+        <v>0.5</v>
       </c>
       <c r="AL25" s="31"/>
       <c r="AM25" s="1" t="n">
@@ -7817,7 +7901,7 @@
         <v> José Raúl Capablanca (Cuba) </v>
       </c>
       <c r="D26" s="26" t="n">
-        <v>2.60110529486542</v>
+        <v>1</v>
       </c>
       <c r="E26" s="19" t="n">
         <f aca="false">E8</f>
@@ -7826,34 +7910,34 @@
       <c r="F26" s="19"/>
       <c r="G26" s="27" t="n">
         <f aca="false">M26/$M$36</f>
-        <v>2.6011052929454</v>
+        <v>1.52948640001166</v>
       </c>
       <c r="H26" s="15" t="n">
         <f aca="false">M26*H$23/$M$37</f>
-        <v>18.3971676963551</v>
+        <v>13.1818181818182</v>
       </c>
       <c r="I26" s="42" t="n">
         <f aca="false">LN(G26)*$I$23</f>
-        <v>166.063173130501</v>
+        <v>73.8182478597859</v>
       </c>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20" t="n">
         <f aca="false">D26*O8/O26</f>
-        <v>2.60110529149323</v>
+        <v>1.45</v>
       </c>
       <c r="O26" s="16" t="n">
         <f aca="false">SUM(P26:AK26)</f>
-        <v>14.5000000187985</v>
+        <v>10</v>
       </c>
       <c r="P26" s="32" t="n">
         <f aca="false">IF(AM8=0,0,$D26/($D26+INDEX($D$7:$D$17,AM8)))</f>
-        <v>0.885169302484703</v>
+        <v>0.5</v>
       </c>
       <c r="Q26" s="31" t="n">
         <f aca="false">IF(AN8=0,0,$D26/($D26+INDEX($D$7:$D$17,AN8)))</f>
-        <v>0.403793218531409</v>
+        <v>0.5</v>
       </c>
       <c r="R26" s="31" t="n">
         <f aca="false">IF(AO8=0,0,$D26/($D26+INDEX($D$7:$D$17,AO8)))</f>
@@ -7861,43 +7945,43 @@
       </c>
       <c r="S26" s="31" t="n">
         <f aca="false">IF(AP8=0,0,$D26/($D26+INDEX($D$7:$D$17,AP8)))</f>
-        <v>0.635561212397342</v>
+        <v>0.5</v>
       </c>
       <c r="T26" s="31" t="n">
         <f aca="false">IF(AQ8=0,0,$D26/($D26+INDEX($D$7:$D$17,AQ8)))</f>
-        <v>0.68188710828467</v>
+        <v>0.5</v>
       </c>
       <c r="U26" s="31" t="n">
         <f aca="false">IF(AR8=0,0,$D26/($D26+INDEX($D$7:$D$17,AR8)))</f>
-        <v>0.703509927845828</v>
+        <v>0.5</v>
       </c>
       <c r="V26" s="31" t="n">
         <f aca="false">IF(AS8=0,0,$D26/($D26+INDEX($D$7:$D$17,AS8)))</f>
-        <v>0.724158201873356</v>
+        <v>0.5</v>
       </c>
       <c r="W26" s="31" t="n">
         <f aca="false">IF(AT8=0,0,$D26/($D26+INDEX($D$7:$D$17,AT8)))</f>
-        <v>0.743870735536155</v>
+        <v>0.5</v>
       </c>
       <c r="X26" s="31" t="n">
         <f aca="false">IF(AU8=0,0,$D26/($D26+INDEX($D$7:$D$17,AU8)))</f>
-        <v>0.797772032168712</v>
+        <v>0.5</v>
       </c>
       <c r="Y26" s="31" t="n">
         <f aca="false">IF(AV8=0,0,$D26/($D26+INDEX($D$7:$D$17,AV8)))</f>
-        <v>0.829704725620113</v>
+        <v>0.5</v>
       </c>
       <c r="Z26" s="31" t="n">
         <f aca="false">IF(AW8=0,0,$D26/($D26+INDEX($D$7:$D$17,AW8)))</f>
-        <v>0.844573544656944</v>
+        <v>0.5</v>
       </c>
       <c r="AA26" s="31" t="n">
         <f aca="false">IF(AX8=0,0,$D26/($D26+INDEX($D$7:$D$17,AX8)))</f>
-        <v>0.885169302484703</v>
+        <v>0.5</v>
       </c>
       <c r="AB26" s="31" t="n">
         <f aca="false">IF(AY8=0,0,$D26/($D26+INDEX($D$7:$D$17,AY8)))</f>
-        <v>0.403793218531409</v>
+        <v>0.5</v>
       </c>
       <c r="AC26" s="31" t="n">
         <f aca="false">IF(AZ8=0,0,$D26/($D26+INDEX($D$7:$D$17,AZ8)))</f>
@@ -7905,35 +7989,35 @@
       </c>
       <c r="AD26" s="31" t="n">
         <f aca="false">IF(BA8=0,0,$D26/($D26+INDEX($D$7:$D$17,BA8)))</f>
-        <v>0.635561212397342</v>
+        <v>0.5</v>
       </c>
       <c r="AE26" s="31" t="n">
         <f aca="false">IF(BB8=0,0,$D26/($D26+INDEX($D$7:$D$17,BB8)))</f>
-        <v>0.68188710828467</v>
+        <v>0.5</v>
       </c>
       <c r="AF26" s="31" t="n">
         <f aca="false">IF(BC8=0,0,$D26/($D26+INDEX($D$7:$D$17,BC8)))</f>
-        <v>0.703509927845828</v>
+        <v>0.5</v>
       </c>
       <c r="AG26" s="31" t="n">
         <f aca="false">IF(BD8=0,0,$D26/($D26+INDEX($D$7:$D$17,BD8)))</f>
-        <v>0.724158201873356</v>
+        <v>0.5</v>
       </c>
       <c r="AH26" s="31" t="n">
         <f aca="false">IF(BE8=0,0,$D26/($D26+INDEX($D$7:$D$17,BE8)))</f>
-        <v>0.743870735536155</v>
+        <v>0.5</v>
       </c>
       <c r="AI26" s="31" t="n">
         <f aca="false">IF(BF8=0,0,$D26/($D26+INDEX($D$7:$D$17,BF8)))</f>
-        <v>0.797772032168712</v>
+        <v>0.5</v>
       </c>
       <c r="AJ26" s="31" t="n">
         <f aca="false">IF(BG8=0,0,$D26/($D26+INDEX($D$7:$D$17,BG8)))</f>
-        <v>0.829704725620113</v>
+        <v>0.5</v>
       </c>
       <c r="AK26" s="33" t="n">
         <f aca="false">IF(BH8=0,0,$D26/($D26+INDEX($D$7:$D$17,BH8)))</f>
-        <v>0.844573544656944</v>
+        <v>0.5</v>
       </c>
       <c r="AL26" s="31"/>
       <c r="AM26" s="1" t="n">
@@ -8035,7 +8119,7 @@
         <v> Alexander Alekhine (France) </v>
       </c>
       <c r="D27" s="26" t="n">
-        <v>1.49150646955304</v>
+        <v>1</v>
       </c>
       <c r="E27" s="19" t="n">
         <f aca="false">E9</f>
@@ -8044,42 +8128,42 @@
       <c r="F27" s="19"/>
       <c r="G27" s="27" t="n">
         <f aca="false">M27/$M$36</f>
-        <v>1.49150646829915</v>
+        <v>1.26578184828551</v>
       </c>
       <c r="H27" s="15" t="n">
         <f aca="false">M27*H$23/$M$37</f>
-        <v>10.5491671913159</v>
+        <v>10.9090909090909</v>
       </c>
       <c r="I27" s="42" t="n">
         <f aca="false">LN(G27)*$I$23</f>
-        <v>69.4500564524913</v>
+        <v>40.9435453848459</v>
       </c>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20" t="n">
         <f aca="false">D27*O9/O27</f>
-        <v>1.49150646746646</v>
+        <v>1.2</v>
       </c>
       <c r="O27" s="16" t="n">
         <f aca="false">SUM(P27:AK27)</f>
-        <v>12.0000000167877</v>
+        <v>10</v>
       </c>
       <c r="P27" s="32" t="n">
         <f aca="false">IF(AM9=0,0,$D27/($D27+INDEX($D$7:$D$17,AM9)))</f>
-        <v>0.757038175101964</v>
+        <v>0.5</v>
       </c>
       <c r="Q27" s="31" t="n">
         <f aca="false">IF(AN9=0,0,$D27/($D27+INDEX($D$7:$D$17,AN9)))</f>
-        <v>0.81550275591784</v>
+        <v>0.5</v>
       </c>
       <c r="R27" s="31" t="n">
         <f aca="false">IF(AO9=0,0,$D27/($D27+INDEX($D$7:$D$17,AO9)))</f>
-        <v>0.279723318915325</v>
+        <v>0.5</v>
       </c>
       <c r="S27" s="31" t="n">
         <f aca="false">IF(AP9=0,0,$D27/($D27+INDEX($D$7:$D$17,AP9)))</f>
-        <v>0.364438787602658</v>
+        <v>0.5</v>
       </c>
       <c r="T27" s="31" t="n">
         <f aca="false">IF(AQ9=0,0,$D27/($D27+INDEX($D$7:$D$17,AQ9)))</f>
@@ -8087,43 +8171,43 @@
       </c>
       <c r="U27" s="31" t="n">
         <f aca="false">IF(AR9=0,0,$D27/($D27+INDEX($D$7:$D$17,AR9)))</f>
-        <v>0.551394831835409</v>
+        <v>0.5</v>
       </c>
       <c r="V27" s="31" t="n">
         <f aca="false">IF(AS9=0,0,$D27/($D27+INDEX($D$7:$D$17,AS9)))</f>
-        <v>0.576377096901331</v>
+        <v>0.5</v>
       </c>
       <c r="W27" s="31" t="n">
         <f aca="false">IF(AT9=0,0,$D27/($D27+INDEX($D$7:$D$17,AT9)))</f>
-        <v>0.600855884056862</v>
+        <v>0.5</v>
       </c>
       <c r="X27" s="31" t="n">
         <f aca="false">IF(AU9=0,0,$D27/($D27+INDEX($D$7:$D$17,AU9)))</f>
-        <v>0.624814729721233</v>
+        <v>0.5</v>
       </c>
       <c r="Y27" s="31" t="n">
         <f aca="false">IF(AV9=0,0,$D27/($D27+INDEX($D$7:$D$17,AV9)))</f>
-        <v>0.693445577860386</v>
+        <v>0.5</v>
       </c>
       <c r="Z27" s="31" t="n">
         <f aca="false">IF(AW9=0,0,$D27/($D27+INDEX($D$7:$D$17,AW9)))</f>
-        <v>0.736408850480833</v>
+        <v>0.5</v>
       </c>
       <c r="AA27" s="31" t="n">
         <f aca="false">IF(AX9=0,0,$D27/($D27+INDEX($D$7:$D$17,AX9)))</f>
-        <v>0.757038175101964</v>
+        <v>0.5</v>
       </c>
       <c r="AB27" s="31" t="n">
         <f aca="false">IF(AY9=0,0,$D27/($D27+INDEX($D$7:$D$17,AY9)))</f>
-        <v>0.81550275591784</v>
+        <v>0.5</v>
       </c>
       <c r="AC27" s="31" t="n">
         <f aca="false">IF(AZ9=0,0,$D27/($D27+INDEX($D$7:$D$17,AZ9)))</f>
-        <v>0.279723318915325</v>
+        <v>0.5</v>
       </c>
       <c r="AD27" s="31" t="n">
         <f aca="false">IF(BA9=0,0,$D27/($D27+INDEX($D$7:$D$17,BA9)))</f>
-        <v>0.364438787602658</v>
+        <v>0.5</v>
       </c>
       <c r="AE27" s="31" t="n">
         <f aca="false">IF(BB9=0,0,$D27/($D27+INDEX($D$7:$D$17,BB9)))</f>
@@ -8131,27 +8215,27 @@
       </c>
       <c r="AF27" s="31" t="n">
         <f aca="false">IF(BC9=0,0,$D27/($D27+INDEX($D$7:$D$17,BC9)))</f>
-        <v>0.551394831835409</v>
+        <v>0.5</v>
       </c>
       <c r="AG27" s="31" t="n">
         <f aca="false">IF(BD9=0,0,$D27/($D27+INDEX($D$7:$D$17,BD9)))</f>
-        <v>0.576377096901331</v>
+        <v>0.5</v>
       </c>
       <c r="AH27" s="31" t="n">
         <f aca="false">IF(BE9=0,0,$D27/($D27+INDEX($D$7:$D$17,BE9)))</f>
-        <v>0.600855884056862</v>
+        <v>0.5</v>
       </c>
       <c r="AI27" s="31" t="n">
         <f aca="false">IF(BF9=0,0,$D27/($D27+INDEX($D$7:$D$17,BF9)))</f>
-        <v>0.624814729721233</v>
+        <v>0.5</v>
       </c>
       <c r="AJ27" s="31" t="n">
         <f aca="false">IF(BG9=0,0,$D27/($D27+INDEX($D$7:$D$17,BG9)))</f>
-        <v>0.693445577860386</v>
+        <v>0.5</v>
       </c>
       <c r="AK27" s="33" t="n">
         <f aca="false">IF(BH9=0,0,$D27/($D27+INDEX($D$7:$D$17,BH9)))</f>
-        <v>0.736408850480833</v>
+        <v>0.5</v>
       </c>
       <c r="AL27" s="31"/>
       <c r="AM27" s="1" t="n">
@@ -8253,7 +8337,7 @@
         <v> Frank Marshall (United States) </v>
       </c>
       <c r="D28" s="26" t="n">
-        <v>1.21346351463835</v>
+        <v>1</v>
       </c>
       <c r="E28" s="19" t="n">
         <f aca="false">E10</f>
@@ -8262,50 +8346,50 @@
       <c r="F28" s="19"/>
       <c r="G28" s="27" t="n">
         <f aca="false">M28/$M$36</f>
-        <v>1.21346351357423</v>
+        <v>1.16030002759505</v>
       </c>
       <c r="H28" s="15" t="n">
         <f aca="false">M28*H$23/$M$37</f>
-        <v>8.58261747926171</v>
+        <v>10</v>
       </c>
       <c r="I28" s="42" t="n">
         <f aca="false">LN(G28)*$I$23</f>
-        <v>33.6106889984212</v>
+        <v>25.828121029086</v>
       </c>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20" t="n">
         <f aca="false">D28*O10/O28</f>
-        <v>1.21346351289676</v>
+        <v>1.1</v>
       </c>
       <c r="O28" s="16" t="n">
         <f aca="false">SUM(P28:AK28)</f>
-        <v>11.0000000157874</v>
+        <v>10</v>
       </c>
       <c r="P28" s="32" t="n">
         <f aca="false">IF(AM10=0,0,$D28/($D28+INDEX($D$7:$D$17,AM10)))</f>
-        <v>0.694465176436714</v>
+        <v>0.5</v>
       </c>
       <c r="Q28" s="31" t="n">
         <f aca="false">IF(AN10=0,0,$D28/($D28+INDEX($D$7:$D$17,AN10)))</f>
-        <v>0.717116136653935</v>
+        <v>0.5</v>
       </c>
       <c r="R28" s="31" t="n">
         <f aca="false">IF(AO10=0,0,$D28/($D28+INDEX($D$7:$D$17,AO10)))</f>
-        <v>0.782426334607822</v>
+        <v>0.5</v>
       </c>
       <c r="S28" s="31" t="n">
         <f aca="false">IF(AP10=0,0,$D28/($D28+INDEX($D$7:$D$17,AP10)))</f>
-        <v>0.240097976576957</v>
+        <v>0.5</v>
       </c>
       <c r="T28" s="31" t="n">
         <f aca="false">IF(AQ10=0,0,$D28/($D28+INDEX($D$7:$D$17,AQ10)))</f>
-        <v>0.31811289171533</v>
+        <v>0.5</v>
       </c>
       <c r="U28" s="31" t="n">
         <f aca="false">IF(AR10=0,0,$D28/($D28+INDEX($D$7:$D$17,AR10)))</f>
-        <v>0.448605168164591</v>
+        <v>0.5</v>
       </c>
       <c r="V28" s="31" t="n">
         <f aca="false">IF(AS10=0,0,$D28/($D28+INDEX($D$7:$D$17,AS10)))</f>
@@ -8313,43 +8397,43 @@
       </c>
       <c r="W28" s="31" t="n">
         <f aca="false">IF(AT10=0,0,$D28/($D28+INDEX($D$7:$D$17,AT10)))</f>
-        <v>0.525380782751302</v>
+        <v>0.5</v>
       </c>
       <c r="X28" s="31" t="n">
         <f aca="false">IF(AU10=0,0,$D28/($D28+INDEX($D$7:$D$17,AU10)))</f>
-        <v>0.550508285188133</v>
+        <v>0.5</v>
       </c>
       <c r="Y28" s="31" t="n">
         <f aca="false">IF(AV10=0,0,$D28/($D28+INDEX($D$7:$D$17,AV10)))</f>
-        <v>0.57535341591413</v>
+        <v>0.5</v>
       </c>
       <c r="Z28" s="31" t="n">
         <f aca="false">IF(AW10=0,0,$D28/($D28+INDEX($D$7:$D$17,AW10)))</f>
-        <v>0.647933839884788</v>
+        <v>0.5</v>
       </c>
       <c r="AA28" s="31" t="n">
         <f aca="false">IF(AX10=0,0,$D28/($D28+INDEX($D$7:$D$17,AX10)))</f>
-        <v>0.694465176436714</v>
+        <v>0.5</v>
       </c>
       <c r="AB28" s="31" t="n">
         <f aca="false">IF(AY10=0,0,$D28/($D28+INDEX($D$7:$D$17,AY10)))</f>
-        <v>0.717116136653935</v>
+        <v>0.5</v>
       </c>
       <c r="AC28" s="31" t="n">
         <f aca="false">IF(AZ10=0,0,$D28/($D28+INDEX($D$7:$D$17,AZ10)))</f>
-        <v>0.782426334607822</v>
+        <v>0.5</v>
       </c>
       <c r="AD28" s="31" t="n">
         <f aca="false">IF(BA10=0,0,$D28/($D28+INDEX($D$7:$D$17,BA10)))</f>
-        <v>0.240097976576957</v>
+        <v>0.5</v>
       </c>
       <c r="AE28" s="31" t="n">
         <f aca="false">IF(BB10=0,0,$D28/($D28+INDEX($D$7:$D$17,BB10)))</f>
-        <v>0.31811289171533</v>
+        <v>0.5</v>
       </c>
       <c r="AF28" s="31" t="n">
         <f aca="false">IF(BC10=0,0,$D28/($D28+INDEX($D$7:$D$17,BC10)))</f>
-        <v>0.448605168164591</v>
+        <v>0.5</v>
       </c>
       <c r="AG28" s="31" t="n">
         <f aca="false">IF(BD10=0,0,$D28/($D28+INDEX($D$7:$D$17,BD10)))</f>
@@ -8357,19 +8441,19 @@
       </c>
       <c r="AH28" s="31" t="n">
         <f aca="false">IF(BE10=0,0,$D28/($D28+INDEX($D$7:$D$17,BE10)))</f>
-        <v>0.525380782751302</v>
+        <v>0.5</v>
       </c>
       <c r="AI28" s="31" t="n">
         <f aca="false">IF(BF10=0,0,$D28/($D28+INDEX($D$7:$D$17,BF10)))</f>
-        <v>0.550508285188133</v>
+        <v>0.5</v>
       </c>
       <c r="AJ28" s="31" t="n">
         <f aca="false">IF(BG10=0,0,$D28/($D28+INDEX($D$7:$D$17,BG10)))</f>
-        <v>0.57535341591413</v>
+        <v>0.5</v>
       </c>
       <c r="AK28" s="33" t="n">
         <f aca="false">IF(BH10=0,0,$D28/($D28+INDEX($D$7:$D$17,BH10)))</f>
-        <v>0.647933839884788</v>
+        <v>0.5</v>
       </c>
       <c r="AL28" s="31"/>
       <c r="AM28" s="1" t="n">
@@ -8471,7 +8555,7 @@
         <v> Richard Réti (Czechoslovakia) </v>
       </c>
       <c r="D29" s="26" t="n">
-        <v>1.09622034605353</v>
+        <v>1</v>
       </c>
       <c r="E29" s="19" t="n">
         <f aca="false">E11</f>
@@ -8480,58 +8564,58 @@
       <c r="F29" s="19"/>
       <c r="G29" s="27" t="n">
         <f aca="false">M29/$M$36</f>
-        <v>1.09622034507466</v>
+        <v>1.10755911724982</v>
       </c>
       <c r="H29" s="15" t="n">
         <f aca="false">M29*H$23/$M$37</f>
-        <v>7.75337683376052</v>
+        <v>9.54545454545455</v>
       </c>
       <c r="I29" s="42" t="n">
         <f aca="false">LN(G29)*$I$23</f>
-        <v>15.9591432038192</v>
+        <v>17.7467665937712</v>
       </c>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20" t="n">
         <f aca="false">D29*O11/O29</f>
-        <v>1.09622034446265</v>
+        <v>1.05</v>
       </c>
       <c r="O29" s="16" t="n">
         <f aca="false">SUM(P29:AK29)</f>
-        <v>10.500000015238</v>
+        <v>10</v>
       </c>
       <c r="P29" s="32" t="n">
         <f aca="false">IF(AM11=0,0,$D29/($D29+INDEX($D$7:$D$17,AM11)))</f>
-        <v>0.624421710295927</v>
+        <v>0.5</v>
       </c>
       <c r="Q29" s="31" t="n">
         <f aca="false">IF(AN11=0,0,$D29/($D29+INDEX($D$7:$D$17,AN11)))</f>
-        <v>0.672489810612375</v>
+        <v>0.5</v>
       </c>
       <c r="R29" s="31" t="n">
         <f aca="false">IF(AO11=0,0,$D29/($D29+INDEX($D$7:$D$17,AO11)))</f>
-        <v>0.696056900886648</v>
+        <v>0.5</v>
       </c>
       <c r="S29" s="31" t="n">
         <f aca="false">IF(AP11=0,0,$D29/($D29+INDEX($D$7:$D$17,AP11)))</f>
-        <v>0.764633331984164</v>
+        <v>0.5</v>
       </c>
       <c r="T29" s="31" t="n">
         <f aca="false">IF(AQ11=0,0,$D29/($D29+INDEX($D$7:$D$17,AQ11)))</f>
-        <v>0.222051170316208</v>
+        <v>0.5</v>
       </c>
       <c r="U29" s="31" t="n">
         <f aca="false">IF(AR11=0,0,$D29/($D29+INDEX($D$7:$D$17,AR11)))</f>
-        <v>0.296490072154172</v>
+        <v>0.5</v>
       </c>
       <c r="V29" s="31" t="n">
         <f aca="false">IF(AS11=0,0,$D29/($D29+INDEX($D$7:$D$17,AS11)))</f>
-        <v>0.423622903098669</v>
+        <v>0.5</v>
       </c>
       <c r="W29" s="31" t="n">
         <f aca="false">IF(AT11=0,0,$D29/($D29+INDEX($D$7:$D$17,AT11)))</f>
-        <v>0.474619217248698</v>
+        <v>0.5</v>
       </c>
       <c r="X29" s="31" t="n">
         <f aca="false">IF(AU11=0,0,$D29/($D29+INDEX($D$7:$D$17,AU11)))</f>
@@ -8539,43 +8623,43 @@
       </c>
       <c r="Y29" s="31" t="n">
         <f aca="false">IF(AV11=0,0,$D29/($D29+INDEX($D$7:$D$17,AV11)))</f>
-        <v>0.525257014325768</v>
+        <v>0.5</v>
       </c>
       <c r="Z29" s="31" t="n">
         <f aca="false">IF(AW11=0,0,$D29/($D29+INDEX($D$7:$D$17,AW11)))</f>
-        <v>0.550357876696386</v>
+        <v>0.5</v>
       </c>
       <c r="AA29" s="31" t="n">
         <f aca="false">IF(AX11=0,0,$D29/($D29+INDEX($D$7:$D$17,AX11)))</f>
-        <v>0.624421710295927</v>
+        <v>0.5</v>
       </c>
       <c r="AB29" s="31" t="n">
         <f aca="false">IF(AY11=0,0,$D29/($D29+INDEX($D$7:$D$17,AY11)))</f>
-        <v>0.672489810612375</v>
+        <v>0.5</v>
       </c>
       <c r="AC29" s="31" t="n">
         <f aca="false">IF(AZ11=0,0,$D29/($D29+INDEX($D$7:$D$17,AZ11)))</f>
-        <v>0.696056900886648</v>
+        <v>0.5</v>
       </c>
       <c r="AD29" s="31" t="n">
         <f aca="false">IF(BA11=0,0,$D29/($D29+INDEX($D$7:$D$17,BA11)))</f>
-        <v>0.764633331984164</v>
+        <v>0.5</v>
       </c>
       <c r="AE29" s="31" t="n">
         <f aca="false">IF(BB11=0,0,$D29/($D29+INDEX($D$7:$D$17,BB11)))</f>
-        <v>0.222051170316208</v>
+        <v>0.5</v>
       </c>
       <c r="AF29" s="31" t="n">
         <f aca="false">IF(BC11=0,0,$D29/($D29+INDEX($D$7:$D$17,BC11)))</f>
-        <v>0.296490072154172</v>
+        <v>0.5</v>
       </c>
       <c r="AG29" s="31" t="n">
         <f aca="false">IF(BD11=0,0,$D29/($D29+INDEX($D$7:$D$17,BD11)))</f>
-        <v>0.423622903098669</v>
+        <v>0.5</v>
       </c>
       <c r="AH29" s="31" t="n">
         <f aca="false">IF(BE11=0,0,$D29/($D29+INDEX($D$7:$D$17,BE11)))</f>
-        <v>0.474619217248698</v>
+        <v>0.5</v>
       </c>
       <c r="AI29" s="31" t="n">
         <f aca="false">IF(BF11=0,0,$D29/($D29+INDEX($D$7:$D$17,BF11)))</f>
@@ -8583,11 +8667,11 @@
       </c>
       <c r="AJ29" s="31" t="n">
         <f aca="false">IF(BG11=0,0,$D29/($D29+INDEX($D$7:$D$17,BG11)))</f>
-        <v>0.525257014325768</v>
+        <v>0.5</v>
       </c>
       <c r="AK29" s="33" t="n">
         <f aca="false">IF(BH11=0,0,$D29/($D29+INDEX($D$7:$D$17,BH11)))</f>
-        <v>0.550357876696386</v>
+        <v>0.5</v>
       </c>
       <c r="AL29" s="31"/>
       <c r="AM29" s="1" t="n">
@@ -8689,7 +8773,7 @@
         <v> Géza Maróczy (Hungary) </v>
       </c>
       <c r="D30" s="26" t="n">
-        <v>0.990796706847064</v>
+        <v>1</v>
       </c>
       <c r="E30" s="19" t="n">
         <f aca="false">E12</f>
@@ -8698,66 +8782,66 @@
       <c r="F30" s="19"/>
       <c r="G30" s="27" t="n">
         <f aca="false">M30/$M$36</f>
-        <v>0.990796705947942</v>
+        <v>1.05481820690459</v>
       </c>
       <c r="H30" s="15" t="n">
         <f aca="false">M30*H$23/$M$37</f>
-        <v>7.00773367451032</v>
+        <v>9.09090909090909</v>
       </c>
       <c r="I30" s="42" t="n">
         <f aca="false">LN(G30)*$I$23</f>
-        <v>-1.60617838434304</v>
+        <v>9.27104696579599</v>
       </c>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20" t="n">
         <f aca="false">D30*O12/O30</f>
-        <v>0.990796705394791</v>
+        <v>1</v>
       </c>
       <c r="O30" s="16" t="n">
         <f aca="false">SUM(P30:AK30)</f>
-        <v>10.0000000146576</v>
+        <v>10</v>
       </c>
       <c r="P30" s="32" t="n">
         <f aca="false">IF(AM12=0,0,$D30/($D30+INDEX($D$7:$D$17,AM12)))</f>
-        <v>0.525229217489307</v>
+        <v>0.5</v>
       </c>
       <c r="Q30" s="31" t="n">
         <f aca="false">IF(AN12=0,0,$D30/($D30+INDEX($D$7:$D$17,AN12)))</f>
-        <v>0.6004270726772</v>
+        <v>0.5</v>
       </c>
       <c r="R30" s="31" t="n">
         <f aca="false">IF(AO12=0,0,$D30/($D30+INDEX($D$7:$D$17,AO12)))</f>
-        <v>0.649844024784691</v>
+        <v>0.5</v>
       </c>
       <c r="S30" s="31" t="n">
         <f aca="false">IF(AP12=0,0,$D30/($D30+INDEX($D$7:$D$17,AP12)))</f>
-        <v>0.674251325752578</v>
+        <v>0.5</v>
       </c>
       <c r="T30" s="31" t="n">
         <f aca="false">IF(AQ12=0,0,$D30/($D30+INDEX($D$7:$D$17,AQ12)))</f>
-        <v>0.745951939020586</v>
+        <v>0.5</v>
       </c>
       <c r="U30" s="31" t="n">
         <f aca="false">IF(AR12=0,0,$D30/($D30+INDEX($D$7:$D$17,AR12)))</f>
-        <v>0.205075813048573</v>
+        <v>0.5</v>
       </c>
       <c r="V30" s="31" t="n">
         <f aca="false">IF(AS12=0,0,$D30/($D30+INDEX($D$7:$D$17,AS12)))</f>
-        <v>0.275841798126644</v>
+        <v>0.5</v>
       </c>
       <c r="W30" s="31" t="n">
         <f aca="false">IF(AT12=0,0,$D30/($D30+INDEX($D$7:$D$17,AT12)))</f>
-        <v>0.399144115943138</v>
+        <v>0.5</v>
       </c>
       <c r="X30" s="31" t="n">
         <f aca="false">IF(AU12=0,0,$D30/($D30+INDEX($D$7:$D$17,AU12)))</f>
-        <v>0.449491714811867</v>
+        <v>0.5</v>
       </c>
       <c r="Y30" s="31" t="n">
         <f aca="false">IF(AV12=0,0,$D30/($D30+INDEX($D$7:$D$17,AV12)))</f>
-        <v>0.474742985674232</v>
+        <v>0.5</v>
       </c>
       <c r="Z30" s="31" t="n">
         <f aca="false">IF(AW12=0,0,$D30/($D30+INDEX($D$7:$D$17,AW12)))</f>
@@ -8765,43 +8849,43 @@
       </c>
       <c r="AA30" s="31" t="n">
         <f aca="false">IF(AX12=0,0,$D30/($D30+INDEX($D$7:$D$17,AX12)))</f>
-        <v>0.525229217489307</v>
+        <v>0.5</v>
       </c>
       <c r="AB30" s="31" t="n">
         <f aca="false">IF(AY12=0,0,$D30/($D30+INDEX($D$7:$D$17,AY12)))</f>
-        <v>0.6004270726772</v>
+        <v>0.5</v>
       </c>
       <c r="AC30" s="31" t="n">
         <f aca="false">IF(AZ12=0,0,$D30/($D30+INDEX($D$7:$D$17,AZ12)))</f>
-        <v>0.649844024784691</v>
+        <v>0.5</v>
       </c>
       <c r="AD30" s="31" t="n">
         <f aca="false">IF(BA12=0,0,$D30/($D30+INDEX($D$7:$D$17,BA12)))</f>
-        <v>0.674251325752578</v>
+        <v>0.5</v>
       </c>
       <c r="AE30" s="31" t="n">
         <f aca="false">IF(BB12=0,0,$D30/($D30+INDEX($D$7:$D$17,BB12)))</f>
-        <v>0.745951939020586</v>
+        <v>0.5</v>
       </c>
       <c r="AF30" s="31" t="n">
         <f aca="false">IF(BC12=0,0,$D30/($D30+INDEX($D$7:$D$17,BC12)))</f>
-        <v>0.205075813048573</v>
+        <v>0.5</v>
       </c>
       <c r="AG30" s="31" t="n">
         <f aca="false">IF(BD12=0,0,$D30/($D30+INDEX($D$7:$D$17,BD12)))</f>
-        <v>0.275841798126644</v>
+        <v>0.5</v>
       </c>
       <c r="AH30" s="31" t="n">
         <f aca="false">IF(BE12=0,0,$D30/($D30+INDEX($D$7:$D$17,BE12)))</f>
-        <v>0.399144115943138</v>
+        <v>0.5</v>
       </c>
       <c r="AI30" s="31" t="n">
         <f aca="false">IF(BF12=0,0,$D30/($D30+INDEX($D$7:$D$17,BF12)))</f>
-        <v>0.449491714811867</v>
+        <v>0.5</v>
       </c>
       <c r="AJ30" s="31" t="n">
         <f aca="false">IF(BG12=0,0,$D30/($D30+INDEX($D$7:$D$17,BG12)))</f>
-        <v>0.474742985674232</v>
+        <v>0.5</v>
       </c>
       <c r="AK30" s="33" t="n">
         <f aca="false">IF(BH12=0,0,$D30/($D30+INDEX($D$7:$D$17,BH12)))</f>
@@ -8907,7 +8991,7 @@
         <v> Efim Bogoljubow (Soviet Union) </v>
       </c>
       <c r="D31" s="26" t="n">
-        <v>0.895611500950775</v>
+        <v>1</v>
       </c>
       <c r="E31" s="19" t="n">
         <f aca="false">E13</f>
@@ -8916,30 +9000,30 @@
       <c r="F31" s="19"/>
       <c r="G31" s="27" t="n">
         <f aca="false">M31/$M$36</f>
-        <v>0.895611500126368</v>
+        <v>1.00207729655936</v>
       </c>
       <c r="H31" s="15" t="n">
         <f aca="false">M31*H$23/$M$37</f>
-        <v>6.33450518258386</v>
+        <v>8.63636363636364</v>
       </c>
       <c r="I31" s="42" t="n">
         <f aca="false">LN(G31)*$I$23</f>
-        <v>-19.1521353943458</v>
+        <v>0.360489081335088</v>
       </c>
       <c r="J31" s="15"/>
       <c r="K31" s="15"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20" t="n">
         <f aca="false">D31*O13/O31</f>
-        <v>0.895611499626358</v>
+        <v>0.95</v>
       </c>
       <c r="O31" s="16" t="n">
         <f aca="false">SUM(P31:AK31)</f>
-        <v>9.50000001404846</v>
+        <v>10</v>
       </c>
       <c r="P31" s="32" t="n">
         <f aca="false">IF(AM13=0,0,$D31/($D31+INDEX($D$7:$D$17,AM13)))</f>
-        <v>0.474770782510694</v>
+        <v>0.5</v>
       </c>
       <c r="Q31" s="31" t="n">
         <f aca="false">IF(AN13=0,0,$D31/($D31+INDEX($D$7:$D$17,AN13)))</f>
@@ -8947,43 +9031,43 @@
       </c>
       <c r="R31" s="31" t="n">
         <f aca="false">IF(AO13=0,0,$D31/($D31+INDEX($D$7:$D$17,AO13)))</f>
-        <v>0.575967772290308</v>
+        <v>0.5</v>
       </c>
       <c r="S31" s="31" t="n">
         <f aca="false">IF(AP13=0,0,$D31/($D31+INDEX($D$7:$D$17,AP13)))</f>
-        <v>0.62652813924141</v>
+        <v>0.5</v>
       </c>
       <c r="T31" s="31" t="n">
         <f aca="false">IF(AQ13=0,0,$D31/($D31+INDEX($D$7:$D$17,AQ13)))</f>
-        <v>0.651689553649636</v>
+        <v>0.5</v>
       </c>
       <c r="U31" s="31" t="n">
         <f aca="false">IF(AR13=0,0,$D31/($D31+INDEX($D$7:$D$17,AR13)))</f>
-        <v>0.726340654991747</v>
+        <v>0.5</v>
       </c>
       <c r="V31" s="31" t="n">
         <f aca="false">IF(AS13=0,0,$D31/($D31+INDEX($D$7:$D$17,AS13)))</f>
-        <v>0.189099862208339</v>
+        <v>0.5</v>
       </c>
       <c r="W31" s="31" t="n">
         <f aca="false">IF(AT13=0,0,$D31/($D31+INDEX($D$7:$D$17,AT13)))</f>
-        <v>0.256129264463845</v>
+        <v>0.5</v>
       </c>
       <c r="X31" s="31" t="n">
         <f aca="false">IF(AU13=0,0,$D31/($D31+INDEX($D$7:$D$17,AU13)))</f>
-        <v>0.375185270278767</v>
+        <v>0.5</v>
       </c>
       <c r="Y31" s="31" t="n">
         <f aca="false">IF(AV13=0,0,$D31/($D31+INDEX($D$7:$D$17,AV13)))</f>
-        <v>0.42464658408587</v>
+        <v>0.5</v>
       </c>
       <c r="Z31" s="31" t="n">
         <f aca="false">IF(AW13=0,0,$D31/($D31+INDEX($D$7:$D$17,AW13)))</f>
-        <v>0.449642123303614</v>
+        <v>0.5</v>
       </c>
       <c r="AA31" s="31" t="n">
         <f aca="false">IF(AX13=0,0,$D31/($D31+INDEX($D$7:$D$17,AX13)))</f>
-        <v>0.474770782510694</v>
+        <v>0.5</v>
       </c>
       <c r="AB31" s="31" t="n">
         <f aca="false">IF(AY13=0,0,$D31/($D31+INDEX($D$7:$D$17,AY13)))</f>
@@ -8991,39 +9075,39 @@
       </c>
       <c r="AC31" s="31" t="n">
         <f aca="false">IF(AZ13=0,0,$D31/($D31+INDEX($D$7:$D$17,AZ13)))</f>
-        <v>0.575967772290308</v>
+        <v>0.5</v>
       </c>
       <c r="AD31" s="31" t="n">
         <f aca="false">IF(BA13=0,0,$D31/($D31+INDEX($D$7:$D$17,BA13)))</f>
-        <v>0.62652813924141</v>
+        <v>0.5</v>
       </c>
       <c r="AE31" s="31" t="n">
         <f aca="false">IF(BB13=0,0,$D31/($D31+INDEX($D$7:$D$17,BB13)))</f>
-        <v>0.651689553649636</v>
+        <v>0.5</v>
       </c>
       <c r="AF31" s="31" t="n">
         <f aca="false">IF(BC13=0,0,$D31/($D31+INDEX($D$7:$D$17,BC13)))</f>
-        <v>0.726340654991747</v>
+        <v>0.5</v>
       </c>
       <c r="AG31" s="31" t="n">
         <f aca="false">IF(BD13=0,0,$D31/($D31+INDEX($D$7:$D$17,BD13)))</f>
-        <v>0.189099862208339</v>
+        <v>0.5</v>
       </c>
       <c r="AH31" s="31" t="n">
         <f aca="false">IF(BE13=0,0,$D31/($D31+INDEX($D$7:$D$17,BE13)))</f>
-        <v>0.256129264463845</v>
+        <v>0.5</v>
       </c>
       <c r="AI31" s="31" t="n">
         <f aca="false">IF(BF13=0,0,$D31/($D31+INDEX($D$7:$D$17,BF13)))</f>
-        <v>0.375185270278767</v>
+        <v>0.5</v>
       </c>
       <c r="AJ31" s="31" t="n">
         <f aca="false">IF(BG13=0,0,$D31/($D31+INDEX($D$7:$D$17,BG13)))</f>
-        <v>0.42464658408587</v>
+        <v>0.5</v>
       </c>
       <c r="AK31" s="33" t="n">
         <f aca="false">IF(BH13=0,0,$D31/($D31+INDEX($D$7:$D$17,BH13)))</f>
-        <v>0.449642123303614</v>
+        <v>0.5</v>
       </c>
       <c r="AL31" s="31"/>
       <c r="AM31" s="1" t="n">
@@ -9125,7 +9209,7 @@
         <v> Savielly Tartakower (Poland) </v>
       </c>
       <c r="D32" s="26" t="n">
-        <v>0.659356578928798</v>
+        <v>1</v>
       </c>
       <c r="E32" s="19" t="n">
         <f aca="false">E14</f>
@@ -9134,38 +9218,38 @@
       <c r="F32" s="19"/>
       <c r="G32" s="27" t="n">
         <f aca="false">M32/$M$36</f>
-        <v>0.659356578301814</v>
+        <v>0.843854565523673</v>
       </c>
       <c r="H32" s="15" t="n">
         <f aca="false">M32*H$23/$M$37</f>
-        <v>4.66351499711011</v>
+        <v>7.27272727272727</v>
       </c>
       <c r="I32" s="42" t="n">
         <f aca="false">LN(G32)*$I$23</f>
-        <v>-72.3518626253056</v>
+        <v>-29.4929582374266</v>
       </c>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20" t="n">
         <f aca="false">D32*O14/O32</f>
-        <v>0.659356577933702</v>
+        <v>0.8</v>
       </c>
       <c r="O32" s="16" t="n">
         <f aca="false">SUM(P32:AK32)</f>
-        <v>8.00000001207354</v>
+        <v>10</v>
       </c>
       <c r="P32" s="32" t="n">
         <f aca="false">IF(AM14=0,0,$D32/($D32+INDEX($D$7:$D$17,AM14)))</f>
-        <v>0.375578289704073</v>
+        <v>0.5</v>
       </c>
       <c r="Q32" s="31" t="n">
         <f aca="false">IF(AN14=0,0,$D32/($D32+INDEX($D$7:$D$17,AN14)))</f>
-        <v>0.3995729273228</v>
+        <v>0.5</v>
       </c>
       <c r="R32" s="31" t="n">
         <f aca="false">IF(AO14=0,0,$D32/($D32+INDEX($D$7:$D$17,AO14)))</f>
-        <v>0.424032227709692</v>
+        <v>0.5</v>
       </c>
       <c r="S32" s="31" t="n">
         <f aca="false">IF(AP14=0,0,$D32/($D32+INDEX($D$7:$D$17,AP14)))</f>
@@ -9173,43 +9257,43 @@
       </c>
       <c r="T32" s="31" t="n">
         <f aca="false">IF(AQ14=0,0,$D32/($D32+INDEX($D$7:$D$17,AQ14)))</f>
-        <v>0.552582054588649</v>
+        <v>0.5</v>
       </c>
       <c r="U32" s="31" t="n">
         <f aca="false">IF(AR14=0,0,$D32/($D32+INDEX($D$7:$D$17,AR14)))</f>
-        <v>0.579380763834809</v>
+        <v>0.5</v>
       </c>
       <c r="V32" s="31" t="n">
         <f aca="false">IF(AS14=0,0,$D32/($D32+INDEX($D$7:$D$17,AS14)))</f>
-        <v>0.6614791577971</v>
+        <v>0.5</v>
       </c>
       <c r="W32" s="31" t="n">
         <f aca="false">IF(AT14=0,0,$D32/($D32+INDEX($D$7:$D$17,AT14)))</f>
-        <v>0.146526034993531</v>
+        <v>0.5</v>
       </c>
       <c r="X32" s="31" t="n">
         <f aca="false">IF(AU14=0,0,$D32/($D32+INDEX($D$7:$D$17,AU14)))</f>
-        <v>0.202227967831288</v>
+        <v>0.5</v>
       </c>
       <c r="Y32" s="31" t="n">
         <f aca="false">IF(AV14=0,0,$D32/($D32+INDEX($D$7:$D$17,AV14)))</f>
-        <v>0.306554422139614</v>
+        <v>0.5</v>
       </c>
       <c r="Z32" s="31" t="n">
         <f aca="false">IF(AW14=0,0,$D32/($D32+INDEX($D$7:$D$17,AW14)))</f>
-        <v>0.352066160115212</v>
+        <v>0.5</v>
       </c>
       <c r="AA32" s="31" t="n">
         <f aca="false">IF(AX14=0,0,$D32/($D32+INDEX($D$7:$D$17,AX14)))</f>
-        <v>0.375578289704073</v>
+        <v>0.5</v>
       </c>
       <c r="AB32" s="31" t="n">
         <f aca="false">IF(AY14=0,0,$D32/($D32+INDEX($D$7:$D$17,AY14)))</f>
-        <v>0.3995729273228</v>
+        <v>0.5</v>
       </c>
       <c r="AC32" s="31" t="n">
         <f aca="false">IF(AZ14=0,0,$D32/($D32+INDEX($D$7:$D$17,AZ14)))</f>
-        <v>0.424032227709692</v>
+        <v>0.5</v>
       </c>
       <c r="AD32" s="31" t="n">
         <f aca="false">IF(BA14=0,0,$D32/($D32+INDEX($D$7:$D$17,BA14)))</f>
@@ -9217,31 +9301,31 @@
       </c>
       <c r="AE32" s="31" t="n">
         <f aca="false">IF(BB14=0,0,$D32/($D32+INDEX($D$7:$D$17,BB14)))</f>
-        <v>0.552582054588649</v>
+        <v>0.5</v>
       </c>
       <c r="AF32" s="31" t="n">
         <f aca="false">IF(BC14=0,0,$D32/($D32+INDEX($D$7:$D$17,BC14)))</f>
-        <v>0.579380763834809</v>
+        <v>0.5</v>
       </c>
       <c r="AG32" s="31" t="n">
         <f aca="false">IF(BD14=0,0,$D32/($D32+INDEX($D$7:$D$17,BD14)))</f>
-        <v>0.6614791577971</v>
+        <v>0.5</v>
       </c>
       <c r="AH32" s="31" t="n">
         <f aca="false">IF(BE14=0,0,$D32/($D32+INDEX($D$7:$D$17,BE14)))</f>
-        <v>0.146526034993531</v>
+        <v>0.5</v>
       </c>
       <c r="AI32" s="31" t="n">
         <f aca="false">IF(BF14=0,0,$D32/($D32+INDEX($D$7:$D$17,BF14)))</f>
-        <v>0.202227967831288</v>
+        <v>0.5</v>
       </c>
       <c r="AJ32" s="31" t="n">
         <f aca="false">IF(BG14=0,0,$D32/($D32+INDEX($D$7:$D$17,BG14)))</f>
-        <v>0.306554422139614</v>
+        <v>0.5</v>
       </c>
       <c r="AK32" s="33" t="n">
         <f aca="false">IF(BH14=0,0,$D32/($D32+INDEX($D$7:$D$17,BH14)))</f>
-        <v>0.352066160115212</v>
+        <v>0.5</v>
       </c>
       <c r="AL32" s="31"/>
       <c r="AM32" s="1" t="n">
@@ -9343,7 +9427,7 @@
         <v> José Raúl Capablanca (Cuba) </v>
       </c>
       <c r="D33" s="26" t="n">
-        <v>0.533871781372612</v>
+        <v>1</v>
       </c>
       <c r="E33" s="19" t="n">
         <f aca="false">E15</f>
@@ -9352,46 +9436,46 @@
       <c r="F33" s="19"/>
       <c r="G33" s="27" t="n">
         <f aca="false">M33/$M$36</f>
-        <v>0.533871780857781</v>
+        <v>0.738372744833214</v>
       </c>
       <c r="H33" s="15" t="n">
         <f aca="false">M33*H$23/$M$37</f>
-        <v>3.77598273604316</v>
+        <v>6.36363636363636</v>
       </c>
       <c r="I33" s="42" t="n">
         <f aca="false">LN(G33)*$I$23</f>
-        <v>-109.025213707138</v>
+        <v>-52.6897370285013</v>
       </c>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20" t="n">
         <f aca="false">D33*O15/O33</f>
-        <v>0.533871780559726</v>
+        <v>0.7</v>
       </c>
       <c r="O33" s="16" t="n">
         <f aca="false">SUM(P33:AK33)</f>
-        <v>7.00000001065837</v>
+        <v>10</v>
       </c>
       <c r="P33" s="32" t="n">
         <f aca="false">IF(AM15=0,0,$D33/($D33+INDEX($D$7:$D$17,AM15)))</f>
-        <v>0.305534823563286</v>
+        <v>0.5</v>
       </c>
       <c r="Q33" s="31" t="n">
         <f aca="false">IF(AN15=0,0,$D33/($D33+INDEX($D$7:$D$17,AN15)))</f>
-        <v>0.327510189387625</v>
+        <v>0.5</v>
       </c>
       <c r="R33" s="31" t="n">
         <f aca="false">IF(AO15=0,0,$D33/($D33+INDEX($D$7:$D$17,AO15)))</f>
-        <v>0.350155975215309</v>
+        <v>0.5</v>
       </c>
       <c r="S33" s="31" t="n">
         <f aca="false">IF(AP15=0,0,$D33/($D33+INDEX($D$7:$D$17,AP15)))</f>
-        <v>0.37347186075859</v>
+        <v>0.5</v>
       </c>
       <c r="T33" s="31" t="n">
         <f aca="false">IF(AQ15=0,0,$D33/($D33+INDEX($D$7:$D$17,AQ15)))</f>
-        <v>0.447417945411351</v>
+        <v>0.5</v>
       </c>
       <c r="U33" s="31" t="n">
         <f aca="false">IF(AR15=0,0,$D33/($D33+INDEX($D$7:$D$17,AR15)))</f>
@@ -9399,43 +9483,43 @@
       </c>
       <c r="V33" s="31" t="n">
         <f aca="false">IF(AS15=0,0,$D33/($D33+INDEX($D$7:$D$17,AS15)))</f>
-        <v>0.527253738055428</v>
+        <v>0.5</v>
       </c>
       <c r="W33" s="31" t="n">
         <f aca="false">IF(AT15=0,0,$D33/($D33+INDEX($D$7:$D$17,AT15)))</f>
-        <v>0.612725675620883</v>
+        <v>0.5</v>
       </c>
       <c r="X33" s="31" t="n">
         <f aca="false">IF(AU15=0,0,$D33/($D33+INDEX($D$7:$D$17,AU15)))</f>
-        <v>0.12204337341766</v>
+        <v>0.5</v>
       </c>
       <c r="Y33" s="31" t="n">
         <f aca="false">IF(AV15=0,0,$D33/($D33+INDEX($D$7:$D$17,AV15)))</f>
-        <v>0.170295274379887</v>
+        <v>0.5</v>
       </c>
       <c r="Z33" s="31" t="n">
         <f aca="false">IF(AW15=0,0,$D33/($D33+INDEX($D$7:$D$17,AW15)))</f>
-        <v>0.263591149519167</v>
+        <v>0.5</v>
       </c>
       <c r="AA33" s="31" t="n">
         <f aca="false">IF(AX15=0,0,$D33/($D33+INDEX($D$7:$D$17,AX15)))</f>
-        <v>0.305534823563286</v>
+        <v>0.5</v>
       </c>
       <c r="AB33" s="31" t="n">
         <f aca="false">IF(AY15=0,0,$D33/($D33+INDEX($D$7:$D$17,AY15)))</f>
-        <v>0.327510189387625</v>
+        <v>0.5</v>
       </c>
       <c r="AC33" s="31" t="n">
         <f aca="false">IF(AZ15=0,0,$D33/($D33+INDEX($D$7:$D$17,AZ15)))</f>
-        <v>0.350155975215309</v>
+        <v>0.5</v>
       </c>
       <c r="AD33" s="31" t="n">
         <f aca="false">IF(BA15=0,0,$D33/($D33+INDEX($D$7:$D$17,BA15)))</f>
-        <v>0.37347186075859</v>
+        <v>0.5</v>
       </c>
       <c r="AE33" s="31" t="n">
         <f aca="false">IF(BB15=0,0,$D33/($D33+INDEX($D$7:$D$17,BB15)))</f>
-        <v>0.447417945411351</v>
+        <v>0.5</v>
       </c>
       <c r="AF33" s="31" t="n">
         <f aca="false">IF(BC15=0,0,$D33/($D33+INDEX($D$7:$D$17,BC15)))</f>
@@ -9443,23 +9527,23 @@
       </c>
       <c r="AG33" s="31" t="n">
         <f aca="false">IF(BD15=0,0,$D33/($D33+INDEX($D$7:$D$17,BD15)))</f>
-        <v>0.527253738055428</v>
+        <v>0.5</v>
       </c>
       <c r="AH33" s="31" t="n">
         <f aca="false">IF(BE15=0,0,$D33/($D33+INDEX($D$7:$D$17,BE15)))</f>
-        <v>0.612725675620883</v>
+        <v>0.5</v>
       </c>
       <c r="AI33" s="31" t="n">
         <f aca="false">IF(BF15=0,0,$D33/($D33+INDEX($D$7:$D$17,BF15)))</f>
-        <v>0.12204337341766</v>
+        <v>0.5</v>
       </c>
       <c r="AJ33" s="31" t="n">
         <f aca="false">IF(BG15=0,0,$D33/($D33+INDEX($D$7:$D$17,BG15)))</f>
-        <v>0.170295274379887</v>
+        <v>0.5</v>
       </c>
       <c r="AK33" s="33" t="n">
         <f aca="false">IF(BH15=0,0,$D33/($D33+INDEX($D$7:$D$17,BH15)))</f>
-        <v>0.263591149519167</v>
+        <v>0.5</v>
       </c>
       <c r="AL33" s="31"/>
       <c r="AM33" s="1" t="n">
@@ -9561,7 +9645,7 @@
         <v> Edward Lasker (United States) </v>
       </c>
       <c r="D34" s="26" t="n">
-        <v>0.478680132136038</v>
+        <v>1</v>
       </c>
       <c r="E34" s="19" t="n">
         <f aca="false">E16</f>
@@ -9570,54 +9654,54 @@
       <c r="F34" s="19"/>
       <c r="G34" s="27" t="n">
         <f aca="false">M34/$M$36</f>
-        <v>0.478680131672165</v>
+        <v>0.685631834487985</v>
       </c>
       <c r="H34" s="15" t="n">
         <f aca="false">M34*H$23/$M$37</f>
-        <v>3.38562175055749</v>
+        <v>5.90909090909091</v>
       </c>
       <c r="I34" s="42" t="n">
         <f aca="false">LN(G34)*$I$23</f>
-        <v>-127.981839271866</v>
+        <v>-65.5636103770618</v>
       </c>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20" t="n">
         <f aca="false">D34*O16/O34</f>
-        <v>0.478680131404923</v>
+        <v>0.65</v>
       </c>
       <c r="O34" s="16" t="n">
         <f aca="false">SUM(P34:AK34)</f>
-        <v>6.50000000992781</v>
+        <v>10</v>
       </c>
       <c r="P34" s="32" t="n">
         <f aca="false">IF(AM16=0,0,$D34/($D34+INDEX($D$7:$D$17,AM16)))</f>
-        <v>0.242961824898036</v>
+        <v>0.5</v>
       </c>
       <c r="Q34" s="31" t="n">
         <f aca="false">IF(AN16=0,0,$D34/($D34+INDEX($D$7:$D$17,AN16)))</f>
-        <v>0.282883863346065</v>
+        <v>0.5</v>
       </c>
       <c r="R34" s="31" t="n">
         <f aca="false">IF(AO16=0,0,$D34/($D34+INDEX($D$7:$D$17,AO16)))</f>
-        <v>0.303943099113352</v>
+        <v>0.5</v>
       </c>
       <c r="S34" s="31" t="n">
         <f aca="false">IF(AP16=0,0,$D34/($D34+INDEX($D$7:$D$17,AP16)))</f>
-        <v>0.325748674247422</v>
+        <v>0.5</v>
       </c>
       <c r="T34" s="31" t="n">
         <f aca="false">IF(AQ16=0,0,$D34/($D34+INDEX($D$7:$D$17,AQ16)))</f>
-        <v>0.348310446350364</v>
+        <v>0.5</v>
       </c>
       <c r="U34" s="31" t="n">
         <f aca="false">IF(AR16=0,0,$D34/($D34+INDEX($D$7:$D$17,AR16)))</f>
-        <v>0.420619236165192</v>
+        <v>0.5</v>
       </c>
       <c r="V34" s="31" t="n">
         <f aca="false">IF(AS16=0,0,$D34/($D34+INDEX($D$7:$D$17,AS16)))</f>
-        <v>0.472746261944572</v>
+        <v>0.5</v>
       </c>
       <c r="W34" s="31" t="n">
         <f aca="false">IF(AT16=0,0,$D34/($D34+INDEX($D$7:$D$17,AT16)))</f>
@@ -9625,43 +9709,43 @@
       </c>
       <c r="X34" s="31" t="n">
         <f aca="false">IF(AU16=0,0,$D34/($D34+INDEX($D$7:$D$17,AU16)))</f>
-        <v>0.586535351824678</v>
+        <v>0.5</v>
       </c>
       <c r="Y34" s="31" t="n">
         <f aca="false">IF(AV16=0,0,$D34/($D34+INDEX($D$7:$D$17,AV16)))</f>
-        <v>0.110824791731169</v>
+        <v>0.5</v>
       </c>
       <c r="Z34" s="31" t="n">
         <f aca="false">IF(AW16=0,0,$D34/($D34+INDEX($D$7:$D$17,AW16)))</f>
-        <v>0.155426455343056</v>
+        <v>0.5</v>
       </c>
       <c r="AA34" s="31" t="n">
         <f aca="false">IF(AX16=0,0,$D34/($D34+INDEX($D$7:$D$17,AX16)))</f>
-        <v>0.242961824898036</v>
+        <v>0.5</v>
       </c>
       <c r="AB34" s="31" t="n">
         <f aca="false">IF(AY16=0,0,$D34/($D34+INDEX($D$7:$D$17,AY16)))</f>
-        <v>0.282883863346065</v>
+        <v>0.5</v>
       </c>
       <c r="AC34" s="31" t="n">
         <f aca="false">IF(AZ16=0,0,$D34/($D34+INDEX($D$7:$D$17,AZ16)))</f>
-        <v>0.303943099113352</v>
+        <v>0.5</v>
       </c>
       <c r="AD34" s="31" t="n">
         <f aca="false">IF(BA16=0,0,$D34/($D34+INDEX($D$7:$D$17,BA16)))</f>
-        <v>0.325748674247422</v>
+        <v>0.5</v>
       </c>
       <c r="AE34" s="31" t="n">
         <f aca="false">IF(BB16=0,0,$D34/($D34+INDEX($D$7:$D$17,BB16)))</f>
-        <v>0.348310446350364</v>
+        <v>0.5</v>
       </c>
       <c r="AF34" s="31" t="n">
         <f aca="false">IF(BC16=0,0,$D34/($D34+INDEX($D$7:$D$17,BC16)))</f>
-        <v>0.420619236165192</v>
+        <v>0.5</v>
       </c>
       <c r="AG34" s="31" t="n">
         <f aca="false">IF(BD16=0,0,$D34/($D34+INDEX($D$7:$D$17,BD16)))</f>
-        <v>0.472746261944572</v>
+        <v>0.5</v>
       </c>
       <c r="AH34" s="31" t="n">
         <f aca="false">IF(BE16=0,0,$D34/($D34+INDEX($D$7:$D$17,BE16)))</f>
@@ -9669,15 +9753,15 @@
       </c>
       <c r="AI34" s="31" t="n">
         <f aca="false">IF(BF16=0,0,$D34/($D34+INDEX($D$7:$D$17,BF16)))</f>
-        <v>0.586535351824678</v>
+        <v>0.5</v>
       </c>
       <c r="AJ34" s="31" t="n">
         <f aca="false">IF(BG16=0,0,$D34/($D34+INDEX($D$7:$D$17,BG16)))</f>
-        <v>0.110824791731169</v>
+        <v>0.5</v>
       </c>
       <c r="AK34" s="33" t="n">
         <f aca="false">IF(BH16=0,0,$D34/($D34+INDEX($D$7:$D$17,BH16)))</f>
-        <v>0.155426455343056</v>
+        <v>0.5</v>
       </c>
       <c r="AL34" s="31"/>
       <c r="AM34" s="1" t="n">
@@ -9779,7 +9863,7 @@
         <v> Dawid Janowski (France) </v>
       </c>
       <c r="D35" s="26" t="n">
-        <v>0.337434583962304</v>
+        <v>1</v>
       </c>
       <c r="E35" s="19" t="n">
         <f aca="false">E17</f>
@@ -9788,62 +9872,62 @@
       <c r="F35" s="19"/>
       <c r="G35" s="27" t="n">
         <f aca="false">M35/$M$36</f>
-        <v>0.33743458363329</v>
+        <v>0.527409103452296</v>
       </c>
       <c r="H35" s="15" t="n">
         <f aca="false">M35*H$23/$M$37</f>
-        <v>2.38661642744261</v>
+        <v>4.54545454545455</v>
       </c>
       <c r="I35" s="42" t="n">
         <f aca="false">LN(G35)*$I$23</f>
-        <v>-188.724163468878</v>
+        <v>-111.140951299796</v>
       </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20" t="n">
         <f aca="false">D35*O17/O35</f>
-        <v>0.337434583444904</v>
+        <v>0.5</v>
       </c>
       <c r="O35" s="16" t="n">
         <f aca="false">SUM(P35:AK35)</f>
-        <v>5.00000000766667</v>
+        <v>10</v>
       </c>
       <c r="P35" s="34" t="n">
         <f aca="false">IF(AM17=0,0,$D35/($D35+INDEX($D$7:$D$17,AM17)))</f>
-        <v>0.114830697515297</v>
+        <v>0.5</v>
       </c>
       <c r="Q35" s="35" t="n">
         <f aca="false">IF(AN17=0,0,$D35/($D35+INDEX($D$7:$D$17,AN17)))</f>
-        <v>0.18449724408216</v>
+        <v>0.5</v>
       </c>
       <c r="R35" s="35" t="n">
         <f aca="false">IF(AO17=0,0,$D35/($D35+INDEX($D$7:$D$17,AO17)))</f>
-        <v>0.217573665392178</v>
+        <v>0.5</v>
       </c>
       <c r="S35" s="35" t="n">
         <f aca="false">IF(AP17=0,0,$D35/($D35+INDEX($D$7:$D$17,AP17)))</f>
-        <v>0.235366668015836</v>
+        <v>0.5</v>
       </c>
       <c r="T35" s="35" t="n">
         <f aca="false">IF(AQ17=0,0,$D35/($D35+INDEX($D$7:$D$17,AQ17)))</f>
-        <v>0.254048060979414</v>
+        <v>0.5</v>
       </c>
       <c r="U35" s="35" t="n">
         <f aca="false">IF(AR17=0,0,$D35/($D35+INDEX($D$7:$D$17,AR17)))</f>
-        <v>0.273659345008253</v>
+        <v>0.5</v>
       </c>
       <c r="V35" s="35" t="n">
         <f aca="false">IF(AS17=0,0,$D35/($D35+INDEX($D$7:$D$17,AS17)))</f>
-        <v>0.3385208422029</v>
+        <v>0.5</v>
       </c>
       <c r="W35" s="35" t="n">
         <f aca="false">IF(AT17=0,0,$D35/($D35+INDEX($D$7:$D$17,AT17)))</f>
-        <v>0.387274324379117</v>
+        <v>0.5</v>
       </c>
       <c r="X35" s="35" t="n">
         <f aca="false">IF(AU17=0,0,$D35/($D35+INDEX($D$7:$D$17,AU17)))</f>
-        <v>0.413464648175322</v>
+        <v>0.5</v>
       </c>
       <c r="Y35" s="35" t="n">
         <f aca="false">IF(AV17=0,0,$D35/($D35+INDEX($D$7:$D$17,AV17)))</f>
@@ -9851,43 +9935,43 @@
       </c>
       <c r="Z35" s="35" t="n">
         <f aca="false">IF(AW17=0,0,$D35/($D35+INDEX($D$7:$D$17,AW17)))</f>
-        <v>0.0807645080828548</v>
+        <v>0.5</v>
       </c>
       <c r="AA35" s="35" t="n">
         <f aca="false">IF(AX17=0,0,$D35/($D35+INDEX($D$7:$D$17,AX17)))</f>
-        <v>0.114830697515297</v>
+        <v>0.5</v>
       </c>
       <c r="AB35" s="35" t="n">
         <f aca="false">IF(AY17=0,0,$D35/($D35+INDEX($D$7:$D$17,AY17)))</f>
-        <v>0.18449724408216</v>
+        <v>0.5</v>
       </c>
       <c r="AC35" s="35" t="n">
         <f aca="false">IF(AZ17=0,0,$D35/($D35+INDEX($D$7:$D$17,AZ17)))</f>
-        <v>0.217573665392178</v>
+        <v>0.5</v>
       </c>
       <c r="AD35" s="35" t="n">
         <f aca="false">IF(BA17=0,0,$D35/($D35+INDEX($D$7:$D$17,BA17)))</f>
-        <v>0.235366668015836</v>
+        <v>0.5</v>
       </c>
       <c r="AE35" s="35" t="n">
         <f aca="false">IF(BB17=0,0,$D35/($D35+INDEX($D$7:$D$17,BB17)))</f>
-        <v>0.254048060979414</v>
+        <v>0.5</v>
       </c>
       <c r="AF35" s="35" t="n">
         <f aca="false">IF(BC17=0,0,$D35/($D35+INDEX($D$7:$D$17,BC17)))</f>
-        <v>0.273659345008253</v>
+        <v>0.5</v>
       </c>
       <c r="AG35" s="35" t="n">
         <f aca="false">IF(BD17=0,0,$D35/($D35+INDEX($D$7:$D$17,BD17)))</f>
-        <v>0.3385208422029</v>
+        <v>0.5</v>
       </c>
       <c r="AH35" s="35" t="n">
         <f aca="false">IF(BE17=0,0,$D35/($D35+INDEX($D$7:$D$17,BE17)))</f>
-        <v>0.387274324379117</v>
+        <v>0.5</v>
       </c>
       <c r="AI35" s="35" t="n">
         <f aca="false">IF(BF17=0,0,$D35/($D35+INDEX($D$7:$D$17,BF17)))</f>
-        <v>0.413464648175322</v>
+        <v>0.5</v>
       </c>
       <c r="AJ35" s="35" t="n">
         <f aca="false">IF(BG17=0,0,$D35/($D35+INDEX($D$7:$D$17,BG17)))</f>
@@ -9895,7 +9979,7 @@
       </c>
       <c r="AK35" s="36" t="n">
         <f aca="false">IF(BH17=0,0,$D35/($D35+INDEX($D$7:$D$17,BH17)))</f>
-        <v>0.0807645080828548</v>
+        <v>0.5</v>
       </c>
       <c r="AL35" s="31"/>
       <c r="AM35" s="1" t="n">
@@ -10011,7 +10095,7 @@
       <c r="L36" s="20"/>
       <c r="M36" s="16" t="n">
         <f aca="false" t="array" ref="M36:M36">EXP(SUM(LN(M25:M35))/$D$5)</f>
-        <v>0.999999999441711</v>
+        <v>0.948030659173529</v>
       </c>
       <c r="O36" s="16" t="n">
         <f aca="false">SUM(O25:O35)</f>
@@ -10023,11 +10107,11 @@
       <c r="L37" s="20"/>
       <c r="M37" s="16" t="n">
         <f aca="false">SUM(M25:M35)</f>
-        <v>14.1386181526658</v>
+        <v>11</v>
       </c>
       <c r="O37" s="43" t="n">
-        <f aca="false" t="array" ref="O37:O37">SUM(IF(P25:AK35=0,1,LN(P25:AK35)*AM25:BH35))</f>
-        <v>-108.367933786706</v>
+        <f aca="false" t="array" ref="O37:O37">SUM(IF(P25:AK35=0,0,LN(P25:AK35)*AM25:BH35))</f>
+        <v>-152.492379723188</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>